<commit_message>
Mini mudancas no Admin e inicio de testes
</commit_message>
<xml_diff>
--- a/sd_checklist_meta1.xlsx
+++ b/sd_checklist_meta1.xlsx
@@ -1,15 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="28109"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="18528"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/raul/Dropbox/Work/Teaching/SD2017/projeto_meta_1/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Bloodeon\Documents\Projects\SD\ProjectSD 17\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="3980" yWindow="1480" windowWidth="27680" windowHeight="19220" tabRatio="500"/>
+    <workbookView xWindow="3975" yWindow="1485" windowWidth="27675" windowHeight="19215" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="2017-2018" sheetId="2" r:id="rId1"/>
@@ -17,7 +17,7 @@
   <definedNames>
     <definedName name="_xlnm.Print_Area" localSheetId="0">'2017-2018'!$A$1:$C$54</definedName>
   </definedNames>
-  <calcPr calcId="150001" concurrentCalc="0"/>
+  <calcPr calcId="171027" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
       <x14:workbookPr defaultImageDpi="32767"/>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="61" uniqueCount="61">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="62">
   <si>
     <t>Requisitos Funcionais</t>
   </si>
@@ -213,12 +213,15 @@
   </si>
   <si>
     <t>Portátil #2 corre 1 servidor RMI , 1 servidor TCP, 1 terminal e 1 consola</t>
+  </si>
+  <si>
+    <t>TESTADO E A FUNCIONAR</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
@@ -631,6 +634,9 @@
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
     </ext>
   </extLst>
 </styleSheet>
@@ -957,32 +963,32 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <sheetPr enableFormatConditionsCalculation="0">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:C60"/>
+  <dimension ref="A1:D60"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="2" ySplit="4" topLeftCell="C5" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="4" topLeftCell="C22" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A6" sqref="A6"/>
-      <selection pane="bottomRight" activeCell="B1" sqref="B1"/>
+      <selection pane="bottomRight" activeCell="D18" sqref="D18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="27.1640625" defaultRowHeight="19" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="27.125" defaultRowHeight="18.75" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="13.5" style="5" customWidth="1"/>
     <col min="2" max="2" width="68" style="2" bestFit="1" customWidth="1"/>
-    <col min="3" max="16384" width="27.1640625" style="5"/>
+    <col min="3" max="16384" width="27.125" style="5"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" s="3" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B1" s="3" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="2" spans="1:3" s="4" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:4" s="4" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B2" s="6" t="s">
         <v>2</v>
       </c>
@@ -990,7 +996,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="3" spans="1:3" s="4" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:4" s="4" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B3" s="6" t="s">
         <v>3</v>
       </c>
@@ -998,7 +1004,7 @@
         <v>2017987654</v>
       </c>
     </row>
-    <row r="4" spans="1:3" s="4" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:4" s="4" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A4" s="4">
         <f>A5+A24+A31+A38</f>
         <v>100</v>
@@ -1011,7 +1017,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="5" spans="1:3" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:4" s="3" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A5" s="3">
         <f>SUM(A6:A23)</f>
         <v>46</v>
@@ -1024,7 +1030,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A6" s="5">
         <v>3</v>
       </c>
@@ -1034,8 +1040,11 @@
       <c r="C6" s="5">
         <v>3</v>
       </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D6" s="5" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A7" s="5">
         <v>3</v>
       </c>
@@ -1046,7 +1055,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A8" s="5">
         <v>3</v>
       </c>
@@ -1057,7 +1066,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A9" s="5">
         <v>3</v>
       </c>
@@ -1068,7 +1077,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A10" s="5">
         <v>3</v>
       </c>
@@ -1079,7 +1088,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A11" s="5">
         <v>3</v>
       </c>
@@ -1090,7 +1099,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A12" s="5">
         <v>3</v>
       </c>
@@ -1101,7 +1110,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A13" s="5">
         <v>3</v>
       </c>
@@ -1112,7 +1121,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A14" s="5">
         <v>3</v>
       </c>
@@ -1123,7 +1132,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A15" s="5">
         <v>3</v>
       </c>
@@ -1134,7 +1143,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A16" s="5">
         <v>3</v>
       </c>
@@ -1145,7 +1154,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A17" s="5">
         <v>3</v>
       </c>
@@ -1156,7 +1165,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A18" s="5">
         <v>5</v>
       </c>
@@ -1167,7 +1176,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A19" s="5">
         <v>5</v>
       </c>
@@ -1178,7 +1187,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A20" s="5">
         <v>0</v>
       </c>
@@ -1186,7 +1195,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A21" s="5">
         <v>0</v>
       </c>
@@ -1194,7 +1203,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A22" s="5">
         <v>0</v>
       </c>
@@ -1202,7 +1211,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A23" s="5">
         <v>0</v>
       </c>
@@ -1210,7 +1219,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="24" spans="1:3" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:3" s="3" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A24" s="3">
         <f>SUM(A25:A30)</f>
         <v>20</v>
@@ -1223,7 +1232,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A25" s="5">
         <v>4</v>
       </c>
@@ -1234,7 +1243,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A26" s="5">
         <v>4</v>
       </c>
@@ -1245,7 +1254,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A27" s="5">
         <v>4</v>
       </c>
@@ -1256,7 +1265,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A28" s="5">
         <v>4</v>
       </c>
@@ -1267,7 +1276,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A29" s="5">
         <v>4</v>
       </c>
@@ -1278,7 +1287,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A30" s="5">
         <v>0</v>
       </c>
@@ -1286,7 +1295,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="31" spans="1:3" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:3" s="3" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A31" s="3">
         <f>SUM(A32:A37)</f>
         <v>24</v>
@@ -1299,7 +1308,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A32" s="5">
         <v>4</v>
       </c>
@@ -1310,7 +1319,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A33" s="5">
         <v>4</v>
       </c>
@@ -1321,7 +1330,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A34" s="5">
         <v>4</v>
       </c>
@@ -1332,7 +1341,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A35" s="5">
         <v>4</v>
       </c>
@@ -1343,7 +1352,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="36" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A36" s="5">
         <v>4</v>
       </c>
@@ -1354,7 +1363,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="37" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A37" s="5">
         <v>4</v>
       </c>
@@ -1365,7 +1374,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="38" spans="1:3" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:3" s="3" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A38" s="3">
         <f>SUM(A39:A43)</f>
         <v>10</v>
@@ -1378,7 +1387,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="39" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A39" s="5">
         <v>2</v>
       </c>
@@ -1389,7 +1398,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="40" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A40" s="5">
         <v>2</v>
       </c>
@@ -1400,7 +1409,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="41" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A41" s="5">
         <v>2</v>
       </c>
@@ -1411,7 +1420,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="42" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A42" s="5">
         <v>2</v>
       </c>
@@ -1422,7 +1431,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="43" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A43" s="5">
         <v>2</v>
       </c>
@@ -1433,7 +1442,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="44" spans="1:3" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:3" s="3" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B44" s="1" t="s">
         <v>8</v>
       </c>
@@ -1442,27 +1451,27 @@
         <v>0</v>
       </c>
     </row>
-    <row r="45" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B45" s="2" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="46" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B46" s="2" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="47" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B47" s="2" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="48" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B48" s="2" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="49" spans="2:3" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="49" spans="2:3" s="3" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B49" s="1" t="s">
         <v>9</v>
       </c>
@@ -1471,57 +1480,57 @@
         <v>0</v>
       </c>
     </row>
-    <row r="50" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="50" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B50" s="2" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="51" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="51" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B51" s="2" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="52" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="52" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B52" s="2" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="53" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="53" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B53" s="2" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="54" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="54" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B54" s="2" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="55" spans="2:3" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="55" spans="2:3" s="3" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B55" s="1" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="56" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="56" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B56" s="8" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="57" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="57" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B57" s="8" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="58" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="58" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B58" s="8" t="s">
         <v>59</v>
       </c>
     </row>
-    <row r="59" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="59" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B59" s="8" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="60" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="60" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B60" s="8" t="s">
         <v>57</v>
       </c>

</xml_diff>

<commit_message>
criacao de cenas e ficheiros a funcionar
</commit_message>
<xml_diff>
--- a/sd_checklist_meta1.xlsx
+++ b/sd_checklist_meta1.xlsx
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="62">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="71" uniqueCount="63">
   <si>
     <t>Requisitos Funcionais</t>
   </si>
@@ -216,6 +216,9 @@
   </si>
   <si>
     <t>TESTADO E A FUNCIONAR</t>
+  </si>
+  <si>
+    <t>x</t>
   </si>
 </sst>
 </file>
@@ -970,10 +973,10 @@
   <dimension ref="A1:D60"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="2" ySplit="4" topLeftCell="C22" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="4" topLeftCell="C5" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A6" sqref="A6"/>
-      <selection pane="bottomRight" activeCell="D18" sqref="D18"/>
+      <selection pane="bottomRight" activeCell="D9" sqref="D9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="27.125" defaultRowHeight="18.75" x14ac:dyDescent="0.3"/>
@@ -1054,6 +1057,9 @@
       <c r="C7" s="5">
         <v>3</v>
       </c>
+      <c r="D7" s="5" t="s">
+        <v>61</v>
+      </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A8" s="5">
@@ -1065,6 +1071,9 @@
       <c r="C8" s="5">
         <v>3</v>
       </c>
+      <c r="D8" s="5" t="s">
+        <v>61</v>
+      </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A9" s="5">
@@ -1076,6 +1085,9 @@
       <c r="C9" s="5">
         <v>3</v>
       </c>
+      <c r="D9" s="5" t="s">
+        <v>61</v>
+      </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A10" s="5">
@@ -1087,6 +1099,9 @@
       <c r="C10" s="5">
         <v>3</v>
       </c>
+      <c r="D10" s="5" t="s">
+        <v>62</v>
+      </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A11" s="5">
@@ -1098,6 +1113,9 @@
       <c r="C11" s="5">
         <v>3</v>
       </c>
+      <c r="D11" s="5" t="s">
+        <v>62</v>
+      </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A12" s="5">
@@ -1109,6 +1127,9 @@
       <c r="C12" s="5">
         <v>3</v>
       </c>
+      <c r="D12" s="5" t="s">
+        <v>62</v>
+      </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A13" s="5">
@@ -1131,6 +1152,9 @@
       <c r="C14" s="5">
         <v>3</v>
       </c>
+      <c r="D14" s="5" t="s">
+        <v>62</v>
+      </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A15" s="5">
@@ -1154,7 +1178,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A17" s="5">
         <v>3</v>
       </c>
@@ -1164,8 +1188,11 @@
       <c r="C17" s="5">
         <v>3</v>
       </c>
-    </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D17" s="5" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A18" s="5">
         <v>5</v>
       </c>
@@ -1175,8 +1202,11 @@
       <c r="C18" s="5">
         <v>5</v>
       </c>
-    </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D18" s="5" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A19" s="5">
         <v>5</v>
       </c>
@@ -1187,7 +1217,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A20" s="5">
         <v>0</v>
       </c>
@@ -1195,7 +1225,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A21" s="5">
         <v>0</v>
       </c>
@@ -1203,7 +1233,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A22" s="5">
         <v>0</v>
       </c>
@@ -1211,7 +1241,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A23" s="5">
         <v>0</v>
       </c>
@@ -1219,7 +1249,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="24" spans="1:3" s="3" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:4" s="3" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A24" s="3">
         <f>SUM(A25:A30)</f>
         <v>20</v>
@@ -1232,7 +1262,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A25" s="5">
         <v>4</v>
       </c>
@@ -1243,7 +1273,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A26" s="5">
         <v>4</v>
       </c>
@@ -1254,7 +1284,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A27" s="5">
         <v>4</v>
       </c>
@@ -1265,7 +1295,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A28" s="5">
         <v>4</v>
       </c>
@@ -1276,7 +1306,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A29" s="5">
         <v>4</v>
       </c>
@@ -1287,7 +1317,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A30" s="5">
         <v>0</v>
       </c>
@@ -1295,7 +1325,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="31" spans="1:3" s="3" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:4" s="3" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A31" s="3">
         <f>SUM(A32:A37)</f>
         <v>24</v>
@@ -1308,7 +1338,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A32" s="5">
         <v>4</v>
       </c>

</xml_diff>